<commit_message>
Cart Model class created
</commit_message>
<xml_diff>
--- a/DB design.xlsx
+++ b/DB design.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aritr\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\Shopping_Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30706C0B-5697-4CC1-A393-B5628D0B4E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8496253A-303F-46F7-A64B-1387B24A5FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -590,7 +590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add userRole column in User table
</commit_message>
<xml_diff>
--- a/DB design.xlsx
+++ b/DB design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\Shopping_Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BACB2117-5A6A-43BA-BFCC-A684FBD2A5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADA5F58-3DAA-4B03-8D5C-E96F940C13FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,14 +216,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -309,11 +301,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -327,10 +318,8 @@
     <xf numFmtId="49" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -616,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -698,9 +687,7 @@
       <c r="B4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
         <v>40</v>
       </c>
@@ -908,7 +895,7 @@
       <c r="F18" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="11" t="s">
         <v>51</v>
       </c>
       <c r="H18" s="11" t="s">
@@ -934,7 +921,9 @@
       <c r="G19" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="H19" s="4"/>
+      <c r="H19" s="11" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>

</xml_diff>

<commit_message>
Address save is not completed
</commit_message>
<xml_diff>
--- a/DB design.xlsx
+++ b/DB design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\Shopping_Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADA5F58-3DAA-4B03-8D5C-E96F940C13FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592315BA-A5C2-477D-81A2-1E134FF50591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
   <si>
     <t>TABLE NAME</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>User Role</t>
+  </si>
+  <si>
+    <t>Image3</t>
+  </si>
+  <si>
+    <t>Image2</t>
   </si>
 </sst>
 </file>
@@ -605,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -975,7 +981,7 @@
         <v>29</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>26</v>
@@ -990,7 +996,9 @@
       <c r="B24" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="4"/>
+      <c r="C24" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="D24" s="4" t="s">
         <v>31</v>
       </c>
@@ -1099,7 +1107,7 @@
         <v>28</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>25</v>
@@ -1114,7 +1122,9 @@
       <c r="B32" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="4"/>
+      <c r="C32" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="D32" s="4" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Excel - updating all user methods
</commit_message>
<xml_diff>
--- a/DB design.xlsx
+++ b/DB design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\Shopping_Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FBF613-43BC-472B-A837-01A209CE760D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D07DCD4-271F-4E71-B606-B906352562A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="69">
   <si>
     <t>TABLE NAME</t>
   </si>
@@ -214,6 +214,24 @@
   </si>
   <si>
     <t>http://localhost:3005/addresses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login </t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chek logged in </t>
+  </si>
+  <si>
+    <t>http://localhost:3005/users/loggedIn</t>
+  </si>
+  <si>
+    <t>http://localhost:3005/users/logout</t>
+  </si>
+  <si>
+    <t>http://localhost:3005/users/login</t>
   </si>
 </sst>
 </file>
@@ -642,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -716,9 +734,15 @@
         <v>40</v>
       </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="F3" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
@@ -730,9 +754,15 @@
         <v>40</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="F4" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
@@ -744,9 +774,15 @@
         <v>40</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="F5" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>

</xml_diff>

<commit_message>
changes in user router methods - new methods added
</commit_message>
<xml_diff>
--- a/DB design.xlsx
+++ b/DB design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\Shopping_Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D07DCD4-271F-4E71-B606-B906352562A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EE0D85-7699-4395-8504-8B5F0EBC6BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="72">
   <si>
     <t>TABLE NAME</t>
   </si>
@@ -102,9 +102,6 @@
     <t>AUTO</t>
   </si>
   <si>
-    <t>ADMIN</t>
-  </si>
-  <si>
     <t>SITE</t>
   </si>
   <si>
@@ -189,9 +186,6 @@
     <t>Image2</t>
   </si>
   <si>
-    <t>UserId</t>
-  </si>
-  <si>
     <t>Addressline</t>
   </si>
   <si>
@@ -232,6 +226,21 @@
   </si>
   <si>
     <t>http://localhost:3005/users/login</t>
+  </si>
+  <si>
+    <t>http://localhost:3005/products/view/{}</t>
+  </si>
+  <si>
+    <t>Get a specific products</t>
+  </si>
+  <si>
+    <t>Edit Profile Page</t>
+  </si>
+  <si>
+    <t>ADMIN DASHBOARD</t>
+  </si>
+  <si>
+    <t>Product Table Product Id</t>
   </si>
 </sst>
 </file>
@@ -269,7 +278,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -302,12 +311,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -327,6 +330,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -358,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -367,12 +394,15 @@
     <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,17 +691,17 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" style="1"/>
@@ -697,101 +727,101 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>51</v>
+      <c r="B2" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="9" t="s">
+      <c r="D2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>45</v>
+      <c r="F2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="4" t="s">
-        <v>33</v>
+      <c r="A3" s="8"/>
+      <c r="B3" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
-        <v>40</v>
+      <c r="D3" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
+      <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="9" t="s">
+      <c r="G5" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>44</v>
+      <c r="H5" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="4" t="s">
-        <v>32</v>
+      <c r="A6" s="8"/>
+      <c r="B6" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="C6" s="4"/>
-      <c r="D6" s="4" t="s">
-        <v>40</v>
+      <c r="D6" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -799,13 +829,13 @@
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="4" t="s">
-        <v>40</v>
+      <c r="D7" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -813,15 +843,15 @@
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>40</v>
+      <c r="D8" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -829,13 +859,13 @@
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="4"/>
       <c r="C9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>40</v>
+      <c r="D9" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -843,13 +873,13 @@
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="4"/>
       <c r="C10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>40</v>
+      <c r="D10" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -857,13 +887,13 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="4"/>
       <c r="C11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>40</v>
+      <c r="D11" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -871,15 +901,15 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10" t="s">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>40</v>
+      <c r="D12" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -887,13 +917,13 @@
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>40</v>
+      <c r="D13" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -901,13 +931,13 @@
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>40</v>
+      <c r="D14" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -915,13 +945,13 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="4"/>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>40</v>
+      <c r="D15" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -935,59 +965,61 @@
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="8"/>
+      <c r="B18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="8"/>
+      <c r="B19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="4" t="s">
-        <v>40</v>
+      <c r="C19" s="12"/>
+      <c r="D19" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -995,13 +1027,13 @@
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="4" t="s">
+      <c r="A20" s="8"/>
+      <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="4" t="s">
-        <v>40</v>
+      <c r="D20" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -1009,13 +1041,13 @@
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="4" t="s">
+      <c r="A21" s="8"/>
+      <c r="B21" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="4" t="s">
-        <v>40</v>
+      <c r="D21" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -1023,13 +1055,13 @@
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="4" t="s">
+      <c r="A22" s="8"/>
+      <c r="B22" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="4" t="s">
-        <v>40</v>
+      <c r="D22" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -1043,64 +1075,66 @@
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>44</v>
+      <c r="D24" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="J24" s="4"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
+      <c r="A25" s="8"/>
       <c r="B25" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="G25" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>45</v>
+      <c r="H25" s="10" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
-      <c r="B26" s="4" t="s">
+      <c r="A26" s="8"/>
+      <c r="B26" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -1108,13 +1142,13 @@
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="9"/>
-      <c r="B27" s="4" t="s">
+      <c r="A27" s="8"/>
+      <c r="B27" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -1122,15 +1156,15 @@
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
+      <c r="A28" s="8"/>
       <c r="B28" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -1138,15 +1172,15 @@
       <c r="H28" s="4"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="9"/>
-      <c r="B29" s="4" t="s">
-        <v>29</v>
+      <c r="A29" s="8"/>
+      <c r="B29" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -1154,15 +1188,15 @@
       <c r="H29" s="4"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="9"/>
-      <c r="B30" s="4" t="s">
+      <c r="A30" s="8"/>
+      <c r="B30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -1176,71 +1210,77 @@
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="H32" s="11" t="s">
+      <c r="F32" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G32" s="10" t="s">
         <v>45</v>
       </c>
+      <c r="H32" s="10" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="8"/>
-      <c r="B33" s="4" t="s">
-        <v>36</v>
+      <c r="A33" s="7"/>
+      <c r="B33" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G33" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H33" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="H33" s="11" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="9"/>
-      <c r="B34" s="4" t="s">
+      <c r="A34" s="8"/>
+      <c r="B34" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
+      <c r="F34" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="9"/>
-      <c r="B35" s="4" t="s">
+      <c r="A35" s="8"/>
+      <c r="B35" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -1248,15 +1288,15 @@
       <c r="H35" s="4"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="9"/>
+      <c r="A36" s="8"/>
       <c r="B36" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -1264,15 +1304,15 @@
       <c r="H36" s="4"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="9"/>
-      <c r="B37" s="4" t="s">
-        <v>28</v>
+      <c r="A37" s="8"/>
+      <c r="B37" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -1280,15 +1320,15 @@
       <c r="H37" s="4"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="9"/>
-      <c r="B38" s="4" t="s">
-        <v>35</v>
+      <c r="A38" s="8"/>
+      <c r="B38" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
@@ -1300,8 +1340,9 @@
     <hyperlink ref="G25" r:id="rId1" xr:uid="{CA800AD6-6C96-4AA0-8577-DC8B41BB3714}"/>
     <hyperlink ref="G24" r:id="rId2" xr:uid="{50BEF9C1-7C82-4869-8B12-9E6A4D582236}"/>
     <hyperlink ref="G17" r:id="rId3" xr:uid="{0AB04B7C-D379-468C-93A1-1AC208E567B9}"/>
+    <hyperlink ref="G34" r:id="rId4" xr:uid="{16317C6B-6CE7-47EE-B502-E1A06314528D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes in cart , image array
</commit_message>
<xml_diff>
--- a/DB design.xlsx
+++ b/DB design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\Shopping_Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EE0D85-7699-4395-8504-8B5F0EBC6BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F330837-34B9-4338-93EF-95E0FAE8C0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="71">
   <si>
     <t>TABLE NAME</t>
   </si>
@@ -114,18 +114,9 @@
     <t>Product Count</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>CALCULATED BY METHODS</t>
-  </si>
-  <si>
     <t>Phone</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>Image1</t>
   </si>
   <si>
@@ -241,6 +232,12 @@
   </si>
   <si>
     <t>Product Table Product Id</t>
+  </si>
+  <si>
+    <t>EmailID</t>
+  </si>
+  <si>
+    <t>need to change to city</t>
   </si>
 </sst>
 </file>
@@ -385,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -403,6 +400,7 @@
     <xf numFmtId="49" fontId="2" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -727,10 +725,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -738,40 +736,40 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" s="3" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -781,17 +779,17 @@
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>65</v>
-      </c>
       <c r="H4" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -801,27 +799,27 @@
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -835,7 +833,7 @@
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -851,7 +849,7 @@
         <v>11</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -865,7 +863,7 @@
         <v>12</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -879,7 +877,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -893,7 +891,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -909,7 +907,7 @@
         <v>11</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -923,7 +921,7 @@
         <v>12</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -937,7 +935,7 @@
         <v>14</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -951,7 +949,7 @@
         <v>13</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -977,49 +975,49 @@
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -1033,7 +1031,7 @@
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -1047,9 +1045,11 @@
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" s="4"/>
+        <v>66</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>70</v>
+      </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -1089,19 +1089,19 @@
         <v>22</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F24" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G24" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G24" s="10" t="s">
-        <v>49</v>
-      </c>
       <c r="H24" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J24" s="4"/>
     </row>
@@ -1118,13 +1118,13 @@
         <v>26</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -1161,7 +1161,7 @@
         <v>21</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>25</v>
@@ -1177,7 +1177,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>25</v>
@@ -1189,15 +1189,11 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
-      <c r="B30" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="B30" s="3"/>
       <c r="C30" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>30</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
@@ -1225,32 +1221,32 @@
         <v>24</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -1260,17 +1256,17 @@
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -1280,7 +1276,7 @@
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -1293,10 +1289,10 @@
         <v>21</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -1309,10 +1305,10 @@
         <v>27</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -1322,13 +1318,13 @@
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="8"/>
       <c r="B38" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>

</xml_diff>

<commit_message>
changes in address and add
</commit_message>
<xml_diff>
--- a/DB design.xlsx
+++ b/DB design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\Shopping_Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0786B2D6-953C-4B89-BE89-73493F7A4E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDC5B4A-35A6-4868-AE69-9BD5BAF99E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="77">
   <si>
     <t>TABLE NAME</t>
   </si>
@@ -237,13 +237,25 @@
     <t>EmailID</t>
   </si>
   <si>
-    <t>need to change to city</t>
-  </si>
-  <si>
     <t>http://localhost:3005/users/rivu@rivu.com</t>
   </si>
   <si>
     <t>Get a specifcuser details</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Update Adress</t>
+  </si>
+  <si>
+    <t>Update User</t>
+  </si>
+  <si>
+    <t>Add A product</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> need to implement in frontend</t>
   </si>
 </sst>
 </file>
@@ -388,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -406,7 +418,6 @@
     <xf numFmtId="49" fontId="2" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,7 +706,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD30"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -829,12 +840,14 @@
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="H6" s="4"/>
+        <v>70</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
@@ -846,7 +859,9 @@
         <v>36</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="F7" s="11" t="s">
+        <v>74</v>
+      </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
@@ -1030,7 +1045,9 @@
         <v>66</v>
       </c>
       <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
+      <c r="F19" s="11" t="s">
+        <v>73</v>
+      </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
@@ -1051,15 +1068,13 @@
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="B21" s="3" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="17" t="s">
-        <v>70</v>
-      </c>
+      <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -1277,8 +1292,12 @@
         <v>67</v>
       </c>
       <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
+      <c r="F34" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>76</v>
+      </c>
       <c r="H34" s="4"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
changes in product quantity field and excel
</commit_message>
<xml_diff>
--- a/DB design.xlsx
+++ b/DB design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\Shopping_Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDC5B4A-35A6-4868-AE69-9BD5BAF99E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6646E3BA-0B9A-4C41-B508-35589472307B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="78">
   <si>
     <t>TABLE NAME</t>
   </si>
@@ -51,12 +51,6 @@
     <t>User Name</t>
   </si>
   <si>
-    <t>User Address 1</t>
-  </si>
-  <si>
-    <t>User Address 2</t>
-  </si>
-  <si>
     <t>SUB TABLE</t>
   </si>
   <si>
@@ -69,9 +63,6 @@
     <t>State</t>
   </si>
   <si>
-    <t>District</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
@@ -117,9 +108,6 @@
     <t>Phone</t>
   </si>
   <si>
-    <t>Image1</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -171,12 +159,6 @@
     <t>User Role</t>
   </si>
   <si>
-    <t>Image3</t>
-  </si>
-  <si>
-    <t>Image2</t>
-  </si>
-  <si>
     <t>Addressline</t>
   </si>
   <si>
@@ -256,6 +238,27 @@
   </si>
   <si>
     <t xml:space="preserve"> need to implement in frontend</t>
+  </si>
+  <si>
+    <t>PATCH</t>
+  </si>
+  <si>
+    <t>http://localhost:3005/addresses/edit/{userId}</t>
+  </si>
+  <si>
+    <t>http://localhost:3005/users/edit/{_id}</t>
+  </si>
+  <si>
+    <t>Remove from Cart</t>
+  </si>
+  <si>
+    <t>Update A product</t>
+  </si>
+  <si>
+    <t>Image Array</t>
+  </si>
+  <si>
+    <t>Address Table</t>
   </si>
 </sst>
 </file>
@@ -293,7 +296,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -327,12 +330,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,13 +408,13 @@
     <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,17 +700,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
@@ -730,7 +727,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -742,10 +739,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -753,40 +750,40 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>41</v>
+      <c r="H2" s="9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="13" t="s">
-        <v>36</v>
+      <c r="D3" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>41</v>
+        <v>52</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -795,86 +792,90 @@
         <v>7</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="13" t="s">
-        <v>36</v>
+      <c r="D4" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>40</v>
+        <v>53</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="13" t="s">
-        <v>36</v>
+      <c r="D5" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>40</v>
+        <v>54</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C6" s="4"/>
-      <c r="D6" s="13" t="s">
-        <v>36</v>
+      <c r="D6" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>40</v>
+        <v>65</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="13" t="s">
-        <v>36</v>
+      <c r="D7" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="F7" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="F7" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>66</v>
+        <v>77</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -884,11 +885,11 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>66</v>
+      <c r="C9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -898,11 +899,11 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="4"/>
-      <c r="C10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>66</v>
+      <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -912,11 +913,11 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="4"/>
-      <c r="C11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="16" t="s">
+      <c r="C11" s="3" t="s">
         <v>66</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -925,14 +926,12 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
-      <c r="B12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="9" t="s">
+      <c r="B12" s="11"/>
+      <c r="C12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="16" t="s">
-        <v>66</v>
+      <c r="D12" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -940,226 +939,234 @@
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="A14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>66</v>
+      <c r="B15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="F15" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="A17" s="8"/>
       <c r="B17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="C17" s="4"/>
       <c r="D17" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>41</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="16" t="s">
         <v>66</v>
       </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="E18" s="4"/>
-      <c r="F18" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>40</v>
-      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="16" t="s">
-        <v>66</v>
+        <v>11</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="E19" s="4"/>
-      <c r="F19" s="11" t="s">
-        <v>73</v>
-      </c>
+      <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
-      <c r="B20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
+      <c r="A21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
+      <c r="D22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="8"/>
+      <c r="B24" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="4"/>
+      <c r="D24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="H24" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="J24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
-      <c r="B25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="4"/>
+      <c r="B25" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="D25" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>41</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="C26" s="11"/>
       <c r="D26" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -1167,195 +1174,149 @@
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
-      <c r="B27" s="3" t="s">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
+      <c r="F28" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="8"/>
+      <c r="A29" s="7"/>
       <c r="B29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>49</v>
-      </c>
+      <c r="C29" s="4"/>
       <c r="D29" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
+        <v>61</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>18</v>
+      <c r="A31" s="8"/>
+      <c r="B31" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>33</v>
+        <v>61</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>41</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="H31" s="4"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
-      <c r="B32" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="4"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="D32" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>40</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C33" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="C33" s="11"/>
       <c r="D33" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E33" s="4"/>
-      <c r="F33" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H33" s="10" t="s">
-        <v>40</v>
-      </c>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C34" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="C34" s="11"/>
       <c r="D34" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E34" s="4"/>
-      <c r="F34" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>76</v>
-      </c>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
       <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="8"/>
-      <c r="B35" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="8"/>
-      <c r="B36" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="8"/>
-      <c r="B37" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G25" r:id="rId1" xr:uid="{CA800AD6-6C96-4AA0-8577-DC8B41BB3714}"/>
-    <hyperlink ref="G24" r:id="rId2" xr:uid="{50BEF9C1-7C82-4869-8B12-9E6A4D582236}"/>
-    <hyperlink ref="G17" r:id="rId3" xr:uid="{0AB04B7C-D379-468C-93A1-1AC208E567B9}"/>
-    <hyperlink ref="G33" r:id="rId4" xr:uid="{16317C6B-6CE7-47EE-B502-E1A06314528D}"/>
+    <hyperlink ref="G22" r:id="rId1" xr:uid="{CA800AD6-6C96-4AA0-8577-DC8B41BB3714}"/>
+    <hyperlink ref="G21" r:id="rId2" xr:uid="{50BEF9C1-7C82-4869-8B12-9E6A4D582236}"/>
+    <hyperlink ref="G14" r:id="rId3" xr:uid="{0AB04B7C-D379-468C-93A1-1AC208E567B9}"/>
+    <hyperlink ref="G30" r:id="rId4" xr:uid="{16317C6B-6CE7-47EE-B502-E1A06314528D}"/>
+    <hyperlink ref="G7" r:id="rId5" xr:uid="{116301C3-BFD9-4761-9741-9D2435F65733}"/>
+    <hyperlink ref="G16" r:id="rId6" xr:uid="{4BF3AA4C-0045-4E2E-A3EC-D6CFF4EC5FC2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
address table removed , user table modified
</commit_message>
<xml_diff>
--- a/DB design.xlsx
+++ b/DB design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\Shopping_Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6646E3BA-0B9A-4C41-B508-35589472307B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771B691B-1914-43D2-A7CA-323D3E6E24A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="73">
   <si>
     <t>TABLE NAME</t>
   </si>
@@ -54,9 +54,6 @@
     <t>SUB TABLE</t>
   </si>
   <si>
-    <t>Address</t>
-  </si>
-  <si>
     <t>Zip</t>
   </si>
   <si>
@@ -171,18 +168,6 @@
     <t>http://localhost:3005/users/submitNew</t>
   </si>
   <si>
-    <t>http://localhost:3005/addresses/submitNew</t>
-  </si>
-  <si>
-    <t>Submit a Address</t>
-  </si>
-  <si>
-    <t>Get all the Adress</t>
-  </si>
-  <si>
-    <t>http://localhost:3005/addresses</t>
-  </si>
-  <si>
     <t xml:space="preserve">Login </t>
   </si>
   <si>
@@ -207,9 +192,6 @@
     <t>Get a specific products</t>
   </si>
   <si>
-    <t>Edit Profile Page</t>
-  </si>
-  <si>
     <t>ADMIN DASHBOARD</t>
   </si>
   <si>
@@ -219,18 +201,12 @@
     <t>EmailID</t>
   </si>
   <si>
-    <t>http://localhost:3005/users/rivu@rivu.com</t>
-  </si>
-  <si>
     <t>Get a specifcuser details</t>
   </si>
   <si>
     <t>City</t>
   </si>
   <si>
-    <t>Update Adress</t>
-  </si>
-  <si>
     <t>Update User</t>
   </si>
   <si>
@@ -243,9 +219,6 @@
     <t>PATCH</t>
   </si>
   <si>
-    <t>http://localhost:3005/addresses/edit/{userId}</t>
-  </si>
-  <si>
     <t>http://localhost:3005/users/edit/{_id}</t>
   </si>
   <si>
@@ -258,7 +231,19 @@
     <t>Image Array</t>
   </si>
   <si>
-    <t>Address Table</t>
+    <t>http://localhost:3005/users/{userId}</t>
+  </si>
+  <si>
+    <t>User ID</t>
+  </si>
+  <si>
+    <t>Orders</t>
+  </si>
+  <si>
+    <t>Order ID</t>
+  </si>
+  <si>
+    <t>Cart Table User ID</t>
   </si>
 </sst>
 </file>
@@ -296,7 +281,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -363,12 +348,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -397,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -413,7 +392,6 @@
     <xf numFmtId="49" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -700,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -739,143 +717,141 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
       <c r="B3" s="3" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="4"/>
+        <v>31</v>
+      </c>
       <c r="F3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>57</v>
-      </c>
       <c r="H3" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="3" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="8" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="8" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
-      <c r="B8" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>60</v>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -884,12 +860,12 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>60</v>
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -898,12 +874,12 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>60</v>
+      <c r="B10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -912,12 +888,12 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>60</v>
+      <c r="B11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -926,12 +902,12 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>60</v>
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -939,115 +915,112 @@
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="A14" s="8"/>
       <c r="B14" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C14" s="11"/>
-      <c r="D14" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>37</v>
-      </c>
+      <c r="D14" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="B15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>36</v>
-      </c>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="3" t="s">
+      <c r="A16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="F16" s="8" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
+      <c r="D17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="3" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="15" t="s">
-        <v>60</v>
+      <c r="D18" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+      <c r="F18" s="15" t="s">
+        <v>65</v>
+      </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="15" t="s">
-        <v>60</v>
+      <c r="D19" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -1055,268 +1028,259 @@
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="8"/>
+      <c r="B21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>14</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
-      <c r="B23" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J23" s="4"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
+      <c r="A24" s="7"/>
       <c r="B24" s="3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
+        <v>55</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
-      <c r="B25" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>76</v>
-      </c>
+      <c r="B25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
+      <c r="F25" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="11"/>
+        <v>16</v>
+      </c>
+      <c r="C26" s="4"/>
       <c r="D26" s="4" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+      <c r="F26" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>62</v>
+      </c>
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="4"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="11"/>
       <c r="D28" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>37</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="7"/>
+      <c r="A29" s="8"/>
       <c r="B29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="C29" s="11"/>
       <c r="D29" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H29" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="8"/>
-      <c r="B30" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E30" s="4"/>
-      <c r="F30" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="8"/>
-      <c r="B31" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="H31" s="4"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
-      <c r="B32" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>76</v>
-      </c>
+      <c r="B32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="10" t="s">
-        <v>75</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F32" s="4"/>
       <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C33" s="11"/>
+        <v>15</v>
+      </c>
+      <c r="C33" s="4"/>
       <c r="D33" s="4" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="11"/>
+        <v>16</v>
+      </c>
+      <c r="C34" s="4"/>
       <c r="D34" s="4" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
     </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="8"/>
+      <c r="B35" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="11"/>
+      <c r="D35" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G22" r:id="rId1" xr:uid="{CA800AD6-6C96-4AA0-8577-DC8B41BB3714}"/>
-    <hyperlink ref="G21" r:id="rId2" xr:uid="{50BEF9C1-7C82-4869-8B12-9E6A4D582236}"/>
-    <hyperlink ref="G14" r:id="rId3" xr:uid="{0AB04B7C-D379-468C-93A1-1AC208E567B9}"/>
-    <hyperlink ref="G30" r:id="rId4" xr:uid="{16317C6B-6CE7-47EE-B502-E1A06314528D}"/>
-    <hyperlink ref="G7" r:id="rId5" xr:uid="{116301C3-BFD9-4761-9741-9D2435F65733}"/>
-    <hyperlink ref="G16" r:id="rId6" xr:uid="{4BF3AA4C-0045-4E2E-A3EC-D6CFF4EC5FC2}"/>
+    <hyperlink ref="G17" r:id="rId1" xr:uid="{CA800AD6-6C96-4AA0-8577-DC8B41BB3714}"/>
+    <hyperlink ref="G16" r:id="rId2" xr:uid="{50BEF9C1-7C82-4869-8B12-9E6A4D582236}"/>
+    <hyperlink ref="G25" r:id="rId3" xr:uid="{16317C6B-6CE7-47EE-B502-E1A06314528D}"/>
+    <hyperlink ref="G7" r:id="rId4" xr:uid="{116301C3-BFD9-4761-9741-9D2435F65733}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{1CA19301-69FB-4368-9167-C804BBBD43E6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Order table implement and methods added
</commit_message>
<xml_diff>
--- a/DB design.xlsx
+++ b/DB design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\Shopping_Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771B691B-1914-43D2-A7CA-323D3E6E24A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53272104-DE26-4364-B6AB-CBF2A38609BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="78">
   <si>
     <t>TABLE NAME</t>
   </si>
@@ -240,10 +240,25 @@
     <t>Orders</t>
   </si>
   <si>
-    <t>Order ID</t>
-  </si>
-  <si>
-    <t>Cart Table User ID</t>
+    <t>Submit a order</t>
+  </si>
+  <si>
+    <t>Get all the orders</t>
+  </si>
+  <si>
+    <t>http://localhost:3005/orders/submitNew</t>
+  </si>
+  <si>
+    <t>http://localhost:3005/orders</t>
+  </si>
+  <si>
+    <t>orderId</t>
+  </si>
+  <si>
+    <t>User Table</t>
+  </si>
+  <si>
+    <t>Cart Table</t>
   </si>
 </sst>
 </file>
@@ -678,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1207,13 +1222,20 @@
         <v>70</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F31" s="8"/>
-      <c r="G31" s="9"/>
+      <c r="E31" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>73</v>
+      </c>
       <c r="H31" s="9" t="s">
         <v>36</v>
       </c>
@@ -1221,28 +1243,38 @@
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E32" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F32" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
+      <c r="G32" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
@@ -1261,7 +1293,7 @@
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="8"/>
       <c r="B35" s="3" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="4" t="s">
@@ -1271,6 +1303,118 @@
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="8"/>
+      <c r="B36" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="8"/>
+      <c r="B37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="8"/>
+      <c r="B38" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="8"/>
+      <c r="B39" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="8"/>
+      <c r="B40" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="8"/>
+      <c r="B41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="8"/>
+      <c r="B42" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="8"/>
+      <c r="B43" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1279,8 +1423,9 @@
     <hyperlink ref="G25" r:id="rId3" xr:uid="{16317C6B-6CE7-47EE-B502-E1A06314528D}"/>
     <hyperlink ref="G7" r:id="rId4" xr:uid="{116301C3-BFD9-4761-9741-9D2435F65733}"/>
     <hyperlink ref="G6" r:id="rId5" xr:uid="{1CA19301-69FB-4368-9167-C804BBBD43E6}"/>
+    <hyperlink ref="G31" r:id="rId6" xr:uid="{86CC4D66-F100-49A6-8E02-89B65D334A86}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
excel updated with latest changes
</commit_message>
<xml_diff>
--- a/DB design.xlsx
+++ b/DB design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\Shopping_Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53272104-DE26-4364-B6AB-CBF2A38609BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D087D4-8940-49E7-8501-CA828E29C9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="81">
   <si>
     <t>TABLE NAME</t>
   </si>
@@ -210,12 +210,6 @@
     <t>Update User</t>
   </si>
   <si>
-    <t>Add A product</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> need to implement in frontend</t>
-  </si>
-  <si>
     <t>PATCH</t>
   </si>
   <si>
@@ -225,9 +219,6 @@
     <t>Remove from Cart</t>
   </si>
   <si>
-    <t>Update A product</t>
-  </si>
-  <si>
     <t>Image Array</t>
   </si>
   <si>
@@ -252,13 +243,31 @@
     <t>http://localhost:3005/orders</t>
   </si>
   <si>
-    <t>orderId</t>
-  </si>
-  <si>
     <t>User Table</t>
   </si>
   <si>
     <t>Cart Table</t>
+  </si>
+  <si>
+    <t>http://localhost:3005/orders/orderHistory/{userId}</t>
+  </si>
+  <si>
+    <t>Get orders history of a user</t>
+  </si>
+  <si>
+    <t>Delete a product</t>
+  </si>
+  <si>
+    <t>Add a product</t>
+  </si>
+  <si>
+    <t>ProductDetails[]</t>
+  </si>
+  <si>
+    <t>ProductDetailsId</t>
+  </si>
+  <si>
+    <t>Product Image[]</t>
   </si>
 </sst>
 </file>
@@ -391,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -407,7 +416,6 @@
     <xf numFmtId="49" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,21 +701,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -741,7 +748,7 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="14" t="s">
@@ -833,7 +840,7 @@
         <v>58</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>35</v>
@@ -853,10 +860,10 @@
         <v>60</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1022,11 +1029,13 @@
         <v>21</v>
       </c>
       <c r="E18" s="4"/>
-      <c r="F18" s="15" t="s">
-        <v>65</v>
+      <c r="F18" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
+      <c r="H18" s="9" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
@@ -1045,10 +1054,10 @@
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" s="6" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>21</v>
@@ -1153,28 +1162,26 @@
         <v>55</v>
       </c>
       <c r="E26" s="4"/>
-      <c r="F26" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>62</v>
-      </c>
+      <c r="F26" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
       <c r="B27" s="6" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>55</v>
       </c>
       <c r="E27" s="4"/>
-      <c r="F27" s="10" t="s">
-        <v>66</v>
+      <c r="F27" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -1219,22 +1226,25 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>75</v>
+        <v>67</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>45</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H31" s="9" t="s">
         <v>36</v>
@@ -1243,20 +1253,22 @@
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H32" s="9" t="s">
         <v>35</v>
@@ -1265,23 +1277,33 @@
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="4"/>
       <c r="D33" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
+      <c r="F33" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="4"/>
       <c r="D34" s="4" t="s">
         <v>21</v>
       </c>
@@ -1293,7 +1315,7 @@
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="8"/>
       <c r="B35" s="3" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="4" t="s">
@@ -1307,7 +1329,7 @@
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="8"/>
       <c r="B36" s="3" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4" t="s">
@@ -1321,7 +1343,7 @@
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="8"/>
       <c r="B37" s="3" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4" t="s">
@@ -1335,7 +1357,7 @@
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="8"/>
       <c r="B38" s="3" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4" t="s">
@@ -1349,7 +1371,7 @@
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="8"/>
       <c r="B39" s="3" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4" t="s">
@@ -1363,7 +1385,7 @@
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="8"/>
       <c r="B40" s="3" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4" t="s">
@@ -1373,48 +1395,6 @@
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="8"/>
-      <c r="B41" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="8"/>
-      <c r="B42" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="8"/>
-      <c r="B43" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1424,8 +1404,9 @@
     <hyperlink ref="G7" r:id="rId4" xr:uid="{116301C3-BFD9-4761-9741-9D2435F65733}"/>
     <hyperlink ref="G6" r:id="rId5" xr:uid="{1CA19301-69FB-4368-9167-C804BBBD43E6}"/>
     <hyperlink ref="G31" r:id="rId6" xr:uid="{86CC4D66-F100-49A6-8E02-89B65D334A86}"/>
+    <hyperlink ref="G33" r:id="rId7" xr:uid="{73F90967-9541-4840-8FDA-1D8D2AB8F1CF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>